<commit_message>
ejercicio 4 csi listo
</commit_message>
<xml_diff>
--- a/Ej4/Mediciones/tc_tp2_ej4_integrador.xlsx
+++ b/Ej4/Mediciones/tc_tp2_ej4_integrador.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="H(f)" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>f(kHz)</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>r</t>
+  </si>
+  <si>
+    <t>entrada al circuito</t>
+  </si>
+  <si>
+    <t>entrada a la resistencia</t>
+  </si>
+  <si>
+    <t>m=1-2</t>
+  </si>
+  <si>
+    <t>tension en la resistencia</t>
   </si>
 </sst>
 </file>
@@ -505,765 +517,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>magnitud</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="4.0819335083114604E-2"/>
-          <c:y val="8.3750000000000005E-2"/>
-          <c:w val="0.89140288713910765"/>
-          <c:h val="0.72088764946048411"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Z(f)'!$A$2:$A$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="1">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Z(f)'!$E$2:$E$21</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="1">
-                  <c:v>64.521992535400287</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>72.113282311935748</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>83.253385543675776</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>83.061389821973762</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>83.246202956672022</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>83.53101173896421</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>84.154482138494998</c:v>
-                </c:pt>
-                <c:pt idx="8" formatCode="General">
-                  <c:v>77.380936697825462</c:v>
-                </c:pt>
-                <c:pt idx="9" formatCode="General">
-                  <c:v>84.101999261972026</c:v>
-                </c:pt>
-                <c:pt idx="10" formatCode="General">
-                  <c:v>84.101999261972026</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="General">
-                  <c:v>84.017916137665623</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="General">
-                  <c:v>83.323312577440234</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="General">
-                  <c:v>81.214409067603853</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="General">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15" formatCode="General">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6522-43B4-B825-675E8F30A90E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="376310688"/>
-        <c:axId val="376313968"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="376310688"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="376313968"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="376313968"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="376310688"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Z(f)'!$A$2:$A$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="1">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Z(f)'!$D$2:$D$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="1">
-                  <c:v>78</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1C1E-4C85-BAF0-D0E182AA6C6C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="490982888"/>
-        <c:axId val="490983544"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="490982888"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="490983544"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="490983544"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="490982888"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1605,7 +858,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1958,7 +1211,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2318,7 +1571,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2878,86 +2131,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5023,1038 +4196,6 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6612,83 +4753,6 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E132AEE-4A33-4D87-9792-1CC6AC68AE88}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B4DAA53-D37C-4EF9-92AF-4A43F659EA02}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6765,7 +4829,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7141,8 +5205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7453,10 +5517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7482,47 +5546,17 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5000</v>
-      </c>
-      <c r="B3">
-        <v>2.8</v>
-      </c>
-      <c r="C3">
-        <v>3.66</v>
-      </c>
-      <c r="D3">
-        <v>78</v>
-      </c>
-      <c r="E3" s="1">
-        <f>20*LOG(B3*$H$19/C3)</f>
-        <v>64.521992535400287</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="G3" s="1">
         <f>B3*$H$19</f>
-        <v>6160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2000</v>
-      </c>
-      <c r="B4">
-        <v>3.96</v>
-      </c>
-      <c r="C4">
-        <v>2.16</v>
-      </c>
-      <c r="D4">
-        <v>73</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" ref="E4:E17" si="0">20*LOG(B4*$H$19/C4)</f>
-        <v>72.113282311935748</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="G4" s="1">
-        <f t="shared" ref="G4:G15" si="1">B4*$H$19</f>
-        <v>8712</v>
+        <f t="shared" ref="G4:G15" si="0">B4*$H$19</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -7539,7 +5573,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E4:E17" si="1">20*LOG(B5*$H$19/C5)</f>
         <v>83.253385543675776</v>
       </c>
       <c r="F5" s="2">
@@ -7547,7 +5581,7 @@
         <v>14543.511450381679</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1905.2</v>
       </c>
     </row>
@@ -7565,7 +5599,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>83.061389821973762</v>
       </c>
       <c r="F6" s="2">
@@ -7573,7 +5607,7 @@
         <v>14225.563909774435</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3784</v>
       </c>
     </row>
@@ -7591,7 +5625,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>83.246202956672022</v>
       </c>
       <c r="F7" s="2">
@@ -7599,7 +5633,7 @@
         <v>14531.490015360983</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9460</v>
       </c>
     </row>
@@ -7617,7 +5651,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>83.53101173896421</v>
       </c>
       <c r="F8" s="2">
@@ -7625,7 +5659,7 @@
         <v>15015.873015873016</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28380</v>
       </c>
     </row>
@@ -7643,7 +5677,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84.154482138494998</v>
       </c>
       <c r="F9" s="2">
@@ -7651,35 +5685,14 @@
         <v>16133.333333333334</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26620</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1000</v>
-      </c>
-      <c r="B10">
-        <v>4.2699999999999996</v>
-      </c>
-      <c r="C10">
-        <v>1.27</v>
-      </c>
-      <c r="D10">
-        <v>60</v>
-      </c>
-      <c r="E10" s="2">
-        <f t="shared" si="0"/>
-        <v>77.380936697825462</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="2"/>
-        <v>7396.8503937007863</v>
-      </c>
-      <c r="G10" s="1">
-        <f t="shared" si="1"/>
-        <v>9393.9999999999982</v>
-      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -7695,7 +5708,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84.101999261972026</v>
       </c>
       <c r="F11" s="2">
@@ -7703,7 +5716,7 @@
         <v>16036.144578313253</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26620</v>
       </c>
     </row>
@@ -7721,7 +5734,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84.101999261972026</v>
       </c>
       <c r="F12" s="2">
@@ -7729,7 +5742,7 @@
         <v>16036.144578313253</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26620</v>
       </c>
     </row>
@@ -7747,7 +5760,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84.017916137665623</v>
       </c>
       <c r="F13" s="2">
@@ -7755,7 +5768,7 @@
         <v>15881.656804733728</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26840</v>
       </c>
     </row>
@@ -7773,7 +5786,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>83.323312577440234</v>
       </c>
       <c r="F14" s="2">
@@ -7781,7 +5794,7 @@
         <v>14661.068702290077</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19206</v>
       </c>
     </row>
@@ -7799,7 +5812,7 @@
         <v>44</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>81.214409067603853</v>
       </c>
       <c r="F15" s="2">
@@ -7807,13 +5820,13 @@
         <v>11500.59880239521</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19206</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="2" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F16" s="2" t="e">
@@ -7821,17 +5834,37 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
       <c r="E17" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="F17" s="2" t="e">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
       <c r="G19" t="s">
         <v>10</v>
       </c>
@@ -7839,13 +5872,291 @@
         <v>2200</v>
       </c>
     </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1">
+        <v>9720</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2">
+        <f>B24/C25*$D$20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.01</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="C25">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>-4</v>
+      </c>
+      <c r="E25" s="2">
+        <f>20*LOG(B25/C25*$D$20)</f>
+        <v>82.987987478701783</v>
+      </c>
+      <c r="F25" s="2">
+        <f>B25/C25*$D$20</f>
+        <v>14105.853658536585</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.02</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="e">
+        <f t="shared" ref="E26:E38" si="3">20*LOG(B26/C26*$D$20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F26" s="2" t="e">
+        <f t="shared" ref="F26:F38" si="4">B26/C26*$D$20</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.05</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F27" s="2" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0.1</v>
+      </c>
+      <c r="B28">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="C28">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="3"/>
+        <v>82.809403597126519</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="4"/>
+        <v>13818.795180722891</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.2</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F29" s="2" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.5</v>
+      </c>
+      <c r="B30">
+        <v>0.59</v>
+      </c>
+      <c r="C30">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="3"/>
+        <v>82.999844859824492</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="4"/>
+        <v>14125.123152709359</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="C31">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="3"/>
+        <v>82.993186731646205</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="4"/>
+        <v>14114.299754299755</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>1.2</v>
+      </c>
+      <c r="C32">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="3"/>
+        <v>83.373420549524454</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="4"/>
+        <v>14745.891276864728</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>1.19</v>
+      </c>
+      <c r="C33">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="3"/>
+        <v>83.180777160692841</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="4"/>
+        <v>14422.443890274313</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>1.19</v>
+      </c>
+      <c r="C34">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="3"/>
+        <v>83.15914355140707</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="4"/>
+        <v>14386.567164179103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>20</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F35" s="2" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>100</v>
+      </c>
+      <c r="B36">
+        <v>1.19</v>
+      </c>
+      <c r="C36">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="D36" s="2">
+        <v>10</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="3"/>
+        <v>82.945720292433805</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="4"/>
+        <v>14037.378640776698</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>200</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F37" s="2" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>500</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F38" s="2" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:A15">
-    <sortCondition ref="A2"/>
+  <sortState ref="A24:A38">
+    <sortCondition ref="A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8105,8 +6416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B13:B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>